<commit_message>
PIM-6335: update catalog modeling fixtures
</commit_message>
<xml_diff>
--- a/features/Context/fixtures/family_variant.xlsx
+++ b/features/Context/fixtures/family_variant.xlsx
@@ -49,7 +49,7 @@
     <t xml:space="preserve">variant-attributes_2</t>
   </si>
   <si>
-    <t xml:space="preserve">clothing_color_and_size</t>
+    <t xml:space="preserve">another_clothing_color_and_size</t>
   </si>
   <si>
     <t xml:space="preserve">clothing</t>
@@ -70,13 +70,13 @@
     <t xml:space="preserve">size</t>
   </si>
   <si>
-    <t xml:space="preserve">color,name,image_1,variation_image,composition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">size,EAN,sku,weight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">shoes_size</t>
+    <t xml:space="preserve">color,name,image,variation_image,composition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">size,ean,sku,weight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">another_shoes_size</t>
   </si>
   <si>
     <t xml:space="preserve">shoes</t>
@@ -97,7 +97,7 @@
     <t xml:space="preserve">weight</t>
   </si>
   <si>
-    <t xml:space="preserve">clothing_color_size</t>
+    <t xml:space="preserve">another_clothing_color_size</t>
   </si>
   <si>
     <t xml:space="preserve">Kleidung nach Farbe/Größe</t>
@@ -112,7 +112,7 @@
     <t xml:space="preserve">color,size</t>
   </si>
   <si>
-    <t xml:space="preserve">name,image_1,variation_image,composition</t>
+    <t xml:space="preserve">name,image,variation_image,composition</t>
   </si>
 </sst>
 </file>
@@ -221,13 +221,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="26.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="41.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.38"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="11.52"/>

</xml_diff>

<commit_message>
PIM-6333: Fix fixtures files
</commit_message>
<xml_diff>
--- a/features/Context/fixtures/family_variant.xlsx
+++ b/features/Context/fixtures/family_variant.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="family_variant" sheetId="1" state="visible" r:id="rId2"/>
@@ -70,10 +70,10 @@
     <t xml:space="preserve">size</t>
   </si>
   <si>
-    <t xml:space="preserve">color,name,image_1,variation_image,composition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">size,EAN,sku,weight</t>
+    <t xml:space="preserve">color,name,image,variation_image,composition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">size,ean,sku,weight</t>
   </si>
   <si>
     <t xml:space="preserve">shoes_size</t>
@@ -112,7 +112,7 @@
     <t xml:space="preserve">color,size</t>
   </si>
   <si>
-    <t xml:space="preserve">name,image_1,variation_image,composition</t>
+    <t xml:space="preserve">name,image,variation_image,composition</t>
   </si>
 </sst>
 </file>
@@ -215,22 +215,21 @@
   </sheetPr>
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="26.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="41.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.38"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="11.52"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.3214285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="40.2295918367347"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.0867346938776"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -340,7 +339,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
PIM-6472: Fix wrong family variant codes
</commit_message>
<xml_diff>
--- a/features/Context/fixtures/family_variant.xlsx
+++ b/features/Context/fixtures/family_variant.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="family_variant" sheetId="1" state="visible" r:id="rId2"/>
@@ -49,7 +49,7 @@
     <t xml:space="preserve">variant-attributes_2</t>
   </si>
   <si>
-    <t xml:space="preserve">clothing_color_and_size</t>
+    <t xml:space="preserve">another_clothing_color_and_size</t>
   </si>
   <si>
     <t xml:space="preserve">clothing</t>
@@ -76,7 +76,7 @@
     <t xml:space="preserve">size,ean,sku,weight</t>
   </si>
   <si>
-    <t xml:space="preserve">shoes_size</t>
+    <t xml:space="preserve">another_shoes_size</t>
   </si>
   <si>
     <t xml:space="preserve">shoes</t>
@@ -97,7 +97,7 @@
     <t xml:space="preserve">weight</t>
   </si>
   <si>
-    <t xml:space="preserve">clothing_color_size</t>
+    <t xml:space="preserve">another_clothing_color_size</t>
   </si>
   <si>
     <t xml:space="preserve">Kleidung nach Farbe/Größe</t>
@@ -187,12 +187,8 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -215,21 +211,23 @@
   </sheetPr>
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.3214285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="40.2295918367347"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.0867346938776"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="26.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="39.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17.55"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -320,7 +318,7 @@
       <c r="B4" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="0" t="s">
         <v>26</v>
       </c>
       <c r="D4" s="0" t="s">
@@ -339,7 +337,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>